<commit_message>
ryddet litt i seminaroppgavene og kalenderen
</commit_message>
<xml_diff>
--- a/diverse/tidsplan-H22.xlsx
+++ b/diverse/tidsplan-H22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s14363\Documents\met4git\met4\diverse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7DF7E4-5DD8-4B12-8B69-7C4CD1E8354D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3397063-A4DD-452E-B234-91F2FBEF7A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Uke</t>
   </si>
@@ -81,48 +81,30 @@
     <t>29.08: Dialogbasert undervisning,  Aud MAX</t>
   </si>
   <si>
-    <t>01.09: Oppgaveseminar Aud A. Se \@ref(seminar) for oppgaver.</t>
-  </si>
-  <si>
     <t>08.09: Dialogbasert undervisning Aud A.</t>
   </si>
   <si>
     <t>12.09: **Oversiktsforelesning: Hypotesetesting** i Aud MAX</t>
   </si>
   <si>
-    <t>15.09: Oppgaveseminar Aud A. Se \@ref(seminar) for oppgaver.</t>
-  </si>
-  <si>
     <t>22.09: Dialogbasert undervisning Aud A.</t>
   </si>
   <si>
-    <t>22.09: Oppgaveseminar Aud A. Se \@ref(seminar) for oppgaver.</t>
-  </si>
-  <si>
     <t>13.10: Dialogbasert undervisning Aud A.</t>
   </si>
   <si>
     <t>17.10:  **Oversiktsforelesning: Tidsrekker** i Aud MAX</t>
   </si>
   <si>
-    <t xml:space="preserve"> 20.10: Oppgaveseminar Aud A. Se \@ref(seminar) for oppgaver.</t>
-  </si>
-  <si>
     <t>27.10: Dialogbasert undervisning Aud A.</t>
   </si>
   <si>
     <t>31.10:  **Oversiktsforelesning: Avansert regresjon og maskinlæring** i Aud MAX</t>
   </si>
   <si>
-    <t xml:space="preserve"> 03.11: Oppgaveseminar Aud A. Se \@ref(seminar) for oppgaver.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 07.10: Kontakttime, kursansvarlig tilgjengelig i Aud MAX</t>
   </si>
   <si>
-    <t>10.11: Oppgaveseminar Aud A. Se \@ref(seminar) for oppgaver.</t>
-  </si>
-  <si>
     <t>26.09: **Oversiktsforelesning Regresjon**, Aud MAX</t>
   </si>
   <si>
@@ -130,6 +112,27 @@
   </si>
   <si>
     <t>Avansert regresjon og maskinlæring/Dataøving 4</t>
+  </si>
+  <si>
+    <t>01.09: Oppgaveseminar 1 Aud A. Se \@ref(seminar) for oppgaver.</t>
+  </si>
+  <si>
+    <t>15.09: Oppgaveseminar 2 Aud A. Se \@ref(seminar) for oppgaver.</t>
+  </si>
+  <si>
+    <t>22.09: Oppgaveseminar 3 Aud A. Se \@ref(seminar) for oppgaver.</t>
+  </si>
+  <si>
+    <t>06.10: Oppgaveseminar 4 Aud A. Se \@ref(seminar) for oppgaver.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 20.10: Oppgaveseminar 5 Aud A. Se \@ref(seminar) for oppgaver.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 03.11: Oppgaveseminar  6, Aud A. Se \@ref(seminar) for oppgaver.</t>
+  </si>
+  <si>
+    <t>10.11: Oppgaveseminar 7, Aud A. Se \@ref(seminar) for oppgaver.</t>
   </si>
 </sst>
 </file>
@@ -456,7 +459,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,7 +510,7 @@
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -521,7 +524,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -532,10 +535,10 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -549,7 +552,7 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -560,10 +563,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -577,7 +580,7 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -591,7 +594,7 @@
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -602,10 +605,10 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -613,13 +616,13 @@
         <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -627,13 +630,13 @@
         <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -644,10 +647,10 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>